<commit_message>
set FC upper limit
</commit_message>
<xml_diff>
--- a/slope.xlsx
+++ b/slope.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1915425_ed_ac_uk/Documents/LFCS/Proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="11_AD4DA82427541F7ACA7EB86AB80A0F5E6BE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E57D328-6DD3-4AF1-B014-CBDBD4B8978F}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="11_AD4DA82427541F7ACA7EB86AB80A0F5E6BE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1841B178-C434-45C4-8CF3-520B48C68C7C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>Qubit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -223,7 +224,280 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>127635</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>148900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>19282</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>31124</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{644A3AC0-0491-B446-6DC8-BC89CD146BEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11100435" y="880420"/>
+          <a:ext cx="4692247" cy="3539824"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>168373</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>128169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>439175</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>179606</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CC7F91D-5A6C-5F77-88F7-DBEDCCF4308B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15941773" y="492236"/>
+          <a:ext cx="6443002" cy="4784303"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="图片 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E4814B18-04CD-852C-8929-CC5DC6EF195B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="390525" y="619125"/>
+          <a:ext cx="3848100" cy="2886075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5042672-7735-9FE2-0604-60053CC228A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4419600" y="885825"/>
+          <a:ext cx="3441700" cy="2581275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>440563</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>313563</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A230841C-997D-B32F-8095-D767828E503E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7984363" y="828676"/>
+          <a:ext cx="3987800" cy="2990850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>669163</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76202</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>60105</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41AE5BE5-CBE9-F9AC-229B-B989BC32143A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12327763" y="981077"/>
+          <a:ext cx="3598037" cy="2698528"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -489,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -501,7 +775,7 @@
     <col min="9" max="9" width="14.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,12 +804,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>-0.10780000000000001</v>
+        <v>0.10780000000000001</v>
       </c>
       <c r="C2">
         <v>420</v>
@@ -552,7 +826,7 @@
         <v>3.606495594111804E-3</v>
       </c>
       <c r="G2">
-        <f>SUM(A2)</f>
+        <f t="shared" ref="G2:G8" si="0">SUM(A2)</f>
         <v>12</v>
       </c>
       <c r="H2">
@@ -560,107 +834,122 @@
         <v>3.149066709137089E-2</v>
       </c>
       <c r="I2">
-        <f>(C2*D2+E2*F2)/A2+G2*H2</f>
-        <v>0.44845989748636145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <f>-(C2*D2/C2+E2*F2/(E2)+G2*H2)</f>
+        <v>-0.38299562681682969</v>
+      </c>
+      <c r="J2">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>-8.9260000000000006E-2</v>
+        <v>8.9267700000000005E-2</v>
       </c>
       <c r="C3">
         <v>490</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D8" si="0">LN(1/(1-0.0015))</f>
+        <f t="shared" ref="D3:D8" si="1">LN(1/(1-0.0015))</f>
         <v>1.5011261262671913E-3</v>
       </c>
       <c r="E3">
         <v>70</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F8" si="1">LN(1/(1-0.0036))</f>
+        <f t="shared" ref="F3:F8" si="2">LN(1/(1-0.0036))</f>
         <v>3.606495594111804E-3</v>
       </c>
       <c r="G3">
-        <f>SUM(A3)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H8" si="2">LN(1/(1-0.031))</f>
+        <f t="shared" ref="H3:H8" si="3">LN(1/(1-0.031))</f>
         <v>3.149066709137089E-2</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I8" si="3">(C3*D3+E3*F3)/A3+G3*H3</f>
-        <v>0.51144123166910316</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" ref="I3:I8" si="4">-(C3*D3/C3+E3*F3/(E3)+G3*H3)</f>
+        <v>-0.44597696099957146</v>
+      </c>
+      <c r="J3">
+        <v>0.15939999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>16</v>
       </c>
+      <c r="B4">
+        <v>7.6581999999999997E-2</v>
+      </c>
       <c r="C4">
         <v>560</v>
       </c>
       <c r="D4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5011261262671913E-3</v>
       </c>
       <c r="E4">
         <v>80</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.606495594111804E-3</v>
       </c>
       <c r="G4">
-        <f>SUM(A4)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.149066709137089E-2</v>
       </c>
       <c r="I4">
-        <f t="shared" si="3"/>
-        <v>0.57442256585184492</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>-0.50895829518231328</v>
+      </c>
+      <c r="J4">
+        <v>0.17712</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>18</v>
       </c>
+      <c r="B5">
+        <v>9.8829999999999994E-3</v>
+      </c>
       <c r="C5">
         <v>646</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5011261262671913E-3</v>
       </c>
       <c r="E5">
         <v>94</v>
       </c>
       <c r="F5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.606495594111804E-3</v>
       </c>
       <c r="G5">
-        <f>SUM(A5)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="H5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.149066709137089E-2</v>
       </c>
       <c r="I5">
-        <f t="shared" si="3"/>
-        <v>0.63953967783440469</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>-0.57193962936505505</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>20</v>
       </c>
@@ -668,30 +957,30 @@
         <v>720</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5011261262671913E-3</v>
       </c>
       <c r="E6">
         <v>105</v>
       </c>
       <c r="F6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.606495594111804E-3</v>
       </c>
       <c r="G6">
-        <f>SUM(A6)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="H6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.149066709137089E-2</v>
       </c>
       <c r="I6">
-        <f t="shared" si="3"/>
-        <v>0.70278798424212363</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>-0.63492096354779681</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>22</v>
       </c>
@@ -699,30 +988,30 @@
         <v>794</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5011261262671913E-3</v>
       </c>
       <c r="E7">
         <v>116</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.606495594111804E-3</v>
       </c>
       <c r="G7">
-        <f>SUM(A7)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.149066709137089E-2</v>
       </c>
       <c r="I7">
-        <f t="shared" si="3"/>
-        <v>0.7659877502453013</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>-0.69790229773053858</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>24</v>
       </c>
@@ -730,27 +1019,285 @@
         <v>880</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5011261262671913E-3</v>
       </c>
       <c r="E8">
         <v>130</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.606495594111804E-3</v>
       </c>
       <c r="G8">
-        <f>SUM(A8)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.149066709137089E-2</v>
       </c>
       <c r="I8">
-        <f t="shared" si="3"/>
-        <v>0.83035248595747069</v>
+        <f t="shared" si="4"/>
+        <v>-0.76088363191328046</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>-0.394457</v>
+      </c>
+      <c r="C12">
+        <v>420</v>
+      </c>
+      <c r="D12">
+        <f>LN(1/(1-0.0015))</f>
+        <v>1.5011261262671913E-3</v>
+      </c>
+      <c r="E12">
+        <v>60</v>
+      </c>
+      <c r="F12">
+        <f>LN(1/(1-0.0036))</f>
+        <v>3.606495594111804E-3</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G18" si="5">SUM(A12)</f>
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <f>LN(1/(1-0.031))</f>
+        <v>3.149066709137089E-2</v>
+      </c>
+      <c r="I12">
+        <f>-(C12*D12/C12+E12*F12/(E12)+G12*H12)</f>
+        <v>-0.38299562681682969</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>-8.5878999999999997E-2</v>
+      </c>
+      <c r="C13">
+        <v>490</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ref="D13:D18" si="6">LN(1/(1-0.0015))</f>
+        <v>1.5011261262671913E-3</v>
+      </c>
+      <c r="E13">
+        <v>70</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ref="F13:F18" si="7">LN(1/(1-0.0036))</f>
+        <v>3.606495594111804E-3</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13:H18" si="8">LN(1/(1-0.031))</f>
+        <v>3.149066709137089E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ref="I13:I18" si="9">-(C13*D13/C13+E13*F13/(E13)+G13*H13)</f>
+        <v>-0.44597696099957146</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>-4.3929999999999997E-2</v>
+      </c>
+      <c r="C14">
+        <v>560</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="6"/>
+        <v>1.5011261262671913E-3</v>
+      </c>
+      <c r="E14">
+        <v>80</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="7"/>
+        <v>3.606495594111804E-3</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="8"/>
+        <v>3.149066709137089E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="9"/>
+        <v>-0.50895829518231328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>9.8829999999999994E-3</v>
+      </c>
+      <c r="C15">
+        <v>646</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="6"/>
+        <v>1.5011261262671913E-3</v>
+      </c>
+      <c r="E15">
+        <v>94</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="7"/>
+        <v>3.606495594111804E-3</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="8"/>
+        <v>3.149066709137089E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="9"/>
+        <v>-0.57193962936505505</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>720</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="6"/>
+        <v>1.5011261262671913E-3</v>
+      </c>
+      <c r="E16">
+        <v>105</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="7"/>
+        <v>3.606495594111804E-3</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="8"/>
+        <v>3.149066709137089E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="9"/>
+        <v>-0.63492096354779681</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>22</v>
+      </c>
+      <c r="C17">
+        <v>794</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>1.5011261262671913E-3</v>
+      </c>
+      <c r="E17">
+        <v>116</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>3.606495594111804E-3</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="8"/>
+        <v>3.149066709137089E-2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="9"/>
+        <v>-0.69790229773053858</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>24</v>
+      </c>
+      <c r="C18">
+        <v>880</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="6"/>
+        <v>1.5011261262671913E-3</v>
+      </c>
+      <c r="E18">
+        <v>130</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>3.606495594111804E-3</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="8"/>
+        <v>3.149066709137089E-2</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="9"/>
+        <v>-0.76088363191328046</v>
       </c>
     </row>
   </sheetData>
@@ -764,8 +1311,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FE725CB-C2FB-4E4B-8105-6C26A7911004}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView zoomScale="60" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -774,4 +1321,21 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E9059C-72F9-4C1B-AABC-2CF5DE51EF3D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added FC for large qubit
</commit_message>
<xml_diff>
--- a/slope.xlsx
+++ b/slope.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1915425_ed_ac_uk/Documents/LFCS/Proj/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="182" documentId="11_AD4DA82427541F7ACA7EB86AB80A0F5E6BE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1841B178-C434-45C4-8CF3-520B48C68C7C}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="11_AD4DA82427541F7ACA7EB86AB80A0F5E6BE8DE12" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE71EFC8-C9A0-4748-A029-D7318498F89E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -765,17 +765,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" width="13.75" customWidth="1"/>
-    <col min="9" max="9" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="14.34765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -804,7 +804,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>12</v>
       </c>
@@ -841,7 +841,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>14</v>
       </c>
@@ -878,7 +878,7 @@
         <v>0.15939999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>16</v>
       </c>
@@ -915,7 +915,7 @@
         <v>0.17712</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>18</v>
       </c>
@@ -949,7 +949,7 @@
         <v>-0.57193962936505505</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>20</v>
       </c>
@@ -980,7 +980,7 @@
         <v>-0.63492096354779681</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>22</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>-0.69790229773053858</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>24</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>-0.76088363191328046</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1105,7 +1105,7 @@
         <v>-0.38299562681682969</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>14</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>-0.44597696099957146</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>16</v>
       </c>
@@ -1173,12 +1173,9 @@
         <v>-0.50895829518231328</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>18</v>
-      </c>
-      <c r="B15">
-        <v>9.8829999999999994E-3</v>
       </c>
       <c r="C15">
         <v>646</v>
@@ -1207,7 +1204,7 @@
         <v>-0.57193962936505505</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>20</v>
       </c>
@@ -1238,7 +1235,7 @@
         <v>-0.63492096354779681</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>22</v>
       </c>
@@ -1269,7 +1266,7 @@
         <v>-0.69790229773053858</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>24</v>
       </c>
@@ -1315,7 +1312,7 @@
       <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1327,11 +1324,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E9059C-72F9-4C1B-AABC-2CF5DE51EF3D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.1" x14ac:dyDescent="0.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>